<commit_message>
Ajout nomenclature 4 et 21 postes
</commit_message>
<xml_diff>
--- a/nomenclature/nomenclature_OCS2d_2021_final.xlsx
+++ b/nomenclature/nomenclature_OCS2d_2021_final.xlsx
@@ -5,12 +5,14 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12570" tabRatio="574"/>
+    <workbookView windowHeight="18435" tabRatio="574"/>
   </bookViews>
   <sheets>
     <sheet name="Marque-Page-A5" sheetId="8" r:id="rId1"/>
     <sheet name="CS_HdF_123" sheetId="1" r:id="rId2"/>
     <sheet name="US_HdF_123" sheetId="2" r:id="rId3"/>
+    <sheet name="4P_HdF" sheetId="9" r:id="rId4"/>
+    <sheet name="21P_HdF" sheetId="10" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Marque-Page-A5'!$A$55:$G$131</definedName>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="387">
   <si>
     <r>
       <rPr>
@@ -434,6 +436,9 @@
     <t>CS6.6.0 Autres couverts à dominante herbacée</t>
   </si>
   <si>
+    <t>Légende : usage du sol</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -1544,16 +1549,94 @@
   <si>
     <t>US7.0.0</t>
   </si>
+  <si>
+    <t>CODE_P4</t>
+  </si>
+  <si>
+    <t>LIBELLE_4P</t>
+  </si>
+  <si>
+    <t>Espaces Urbanisés</t>
+  </si>
+  <si>
+    <t>Espaces Agricoles</t>
+  </si>
+  <si>
+    <t>Espaces Naturels, Semi-Naturels</t>
+  </si>
+  <si>
+    <t>Infrastructures</t>
+  </si>
+  <si>
+    <t>CODE_P21</t>
+  </si>
+  <si>
+    <t>LIBELLE_21P</t>
+  </si>
+  <si>
+    <t>Bâti de l’habitat</t>
+  </si>
+  <si>
+    <t>Bâti des exploitations agricoles</t>
+  </si>
+  <si>
+    <t>Bâti commercial</t>
+  </si>
+  <si>
+    <t>Bâti industriel et autres activités économiques</t>
+  </si>
+  <si>
+    <t>Bâti des services et transports</t>
+  </si>
+  <si>
+    <t>Autres bâtis</t>
+  </si>
+  <si>
+    <t>Routes</t>
+  </si>
+  <si>
+    <t>Voies ferrées</t>
+  </si>
+  <si>
+    <t>Zones aéroportuaires</t>
+  </si>
+  <si>
+    <t>Canaux et rivières navigables</t>
+  </si>
+  <si>
+    <t>Espaces non végétalisés de l'habitat</t>
+  </si>
+  <si>
+    <t>Espaces végétalisés de l'habitat</t>
+  </si>
+  <si>
+    <t>Autres espaces artificialisés non végétalisés</t>
+  </si>
+  <si>
+    <t>Autres espaces artificialisés végétalisés</t>
+  </si>
+  <si>
+    <t>Autres terres agricoles</t>
+  </si>
+  <si>
+    <t>Espaces boisés</t>
+  </si>
+  <si>
+    <t>Espaces végétalisés non boisés</t>
+  </si>
+  <si>
+    <t>Espaces non végétalisés</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="35">
     <font>
@@ -1620,36 +1703,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1663,25 +1723,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1704,7 +1747,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1712,6 +1770,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1733,14 +1807,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1754,16 +1821,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2357,7 +2440,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2369,13 +2470,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2387,157 +2614,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2599,17 +2682,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
@@ -2628,24 +2700,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2661,6 +2720,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2694,141 +2762,156 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="104" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="102" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="120" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="110" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="119" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="118" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="117" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="115" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="112" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="109" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="108" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="104" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="91" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="117" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="106" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="105" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="95" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="102" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="100" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="120" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="111" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="112" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="98" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="109" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="121" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="103" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="101" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="107" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="111" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="119" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="92" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="118" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="105" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="110" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="94" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="100" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="101" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="114" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="98" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="96" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="106" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="113" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="103" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="97" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="116" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="107" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="103" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="94" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="116" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="93" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="96" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="97" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="121" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="116" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="113" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="99" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="92" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="93" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="99" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="91" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3588,7 +3671,7 @@
   <dimension ref="A1:G131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -4203,7 +4286,7 @@
     </row>
     <row r="56" spans="2:7">
       <c r="B56" s="6" t="s">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="C56" s="6"/>
       <c r="G56" s="17"/>
@@ -4234,15 +4317,15 @@
     <row r="59" ht="15" customHeight="1" spans="1:7">
       <c r="A59" s="54"/>
       <c r="B59" s="57" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C59" s="16"/>
       <c r="D59" s="56"/>
       <c r="E59" s="94" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F59" s="64" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G59" s="89"/>
     </row>
@@ -4252,7 +4335,7 @@
       <c r="D60" s="17"/>
       <c r="E60" s="94"/>
       <c r="F60" s="64" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G60" s="95"/>
     </row>
@@ -4261,7 +4344,7 @@
       <c r="B61" s="57"/>
       <c r="E61" s="94"/>
       <c r="F61" s="64" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G61" s="56"/>
     </row>
@@ -4270,7 +4353,7 @@
       <c r="B62" s="57"/>
       <c r="E62" s="94"/>
       <c r="F62" s="64" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G62" s="96"/>
     </row>
@@ -4279,7 +4362,7 @@
       <c r="B63" s="57"/>
       <c r="E63" s="94"/>
       <c r="F63" s="64" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G63" s="97"/>
     </row>
@@ -4288,7 +4371,7 @@
       <c r="B64" s="57"/>
       <c r="E64" s="94"/>
       <c r="F64" s="64" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G64" s="98"/>
     </row>
@@ -4297,7 +4380,7 @@
       <c r="B65" s="57"/>
       <c r="E65" s="94"/>
       <c r="F65" s="64" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G65" s="122"/>
     </row>
@@ -4306,10 +4389,10 @@
       <c r="B66" s="57"/>
       <c r="D66" s="99"/>
       <c r="E66" s="94" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F66" s="64" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G66" s="123"/>
     </row>
@@ -4318,7 +4401,7 @@
       <c r="B67" s="57"/>
       <c r="E67" s="94"/>
       <c r="F67" s="64" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G67" s="124"/>
     </row>
@@ -4327,7 +4410,7 @@
       <c r="B68" s="57"/>
       <c r="E68" s="94"/>
       <c r="F68" s="64" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G68" s="125"/>
     </row>
@@ -4336,7 +4419,7 @@
       <c r="B69" s="57"/>
       <c r="E69" s="94"/>
       <c r="F69" s="64" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G69" s="99"/>
     </row>
@@ -4345,10 +4428,10 @@
       <c r="B70" s="57"/>
       <c r="D70" s="100"/>
       <c r="E70" s="94" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F70" s="64" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G70" s="126"/>
     </row>
@@ -4357,7 +4440,7 @@
       <c r="B71" s="57"/>
       <c r="E71" s="94"/>
       <c r="F71" s="64" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G71" s="127"/>
     </row>
@@ -4366,10 +4449,10 @@
       <c r="B72" s="57"/>
       <c r="D72" s="101"/>
       <c r="E72" s="83" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F72" s="64" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G72" s="101"/>
     </row>
@@ -4390,14 +4473,14 @@
     <row r="76" ht="21" spans="1:7">
       <c r="A76" s="102"/>
       <c r="B76" s="103" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D76" s="102"/>
       <c r="E76" s="59" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F76" s="64" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G76" s="102"/>
     </row>
@@ -4406,7 +4489,7 @@
       <c r="B77" s="103"/>
       <c r="E77" s="59"/>
       <c r="F77" s="64" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G77" s="129"/>
     </row>
@@ -4415,7 +4498,7 @@
       <c r="B78" s="103"/>
       <c r="E78" s="59"/>
       <c r="F78" s="64" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G78" s="130"/>
     </row>
@@ -4424,7 +4507,7 @@
       <c r="B79" s="103"/>
       <c r="E79" s="59"/>
       <c r="F79" s="64" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G79" s="131"/>
     </row>
@@ -4433,7 +4516,7 @@
       <c r="B80" s="103"/>
       <c r="E80" s="59"/>
       <c r="F80" s="64" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G80" s="132"/>
     </row>
@@ -4442,10 +4525,10 @@
       <c r="B81" s="103"/>
       <c r="D81" s="104"/>
       <c r="E81" s="83" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F81" s="64" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G81" s="104"/>
     </row>
@@ -4466,14 +4549,14 @@
     <row r="85" ht="21" spans="1:7">
       <c r="A85" s="105"/>
       <c r="B85" s="106" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D85" s="105"/>
       <c r="E85" s="59" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F85" s="64" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G85" s="134"/>
     </row>
@@ -4482,7 +4565,7 @@
       <c r="B86" s="106"/>
       <c r="E86" s="59"/>
       <c r="F86" s="64" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G86" s="135"/>
     </row>
@@ -4491,7 +4574,7 @@
       <c r="B87" s="106"/>
       <c r="E87" s="59"/>
       <c r="F87" s="64" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G87" s="136"/>
     </row>
@@ -4500,7 +4583,7 @@
       <c r="B88" s="106"/>
       <c r="E88" s="59"/>
       <c r="F88" s="64" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G88" s="137"/>
     </row>
@@ -4509,7 +4592,7 @@
       <c r="B89" s="106"/>
       <c r="E89" s="59"/>
       <c r="F89" s="64" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G89" s="138"/>
     </row>
@@ -4518,7 +4601,7 @@
       <c r="B90" s="106"/>
       <c r="E90" s="59"/>
       <c r="F90" s="64" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G90" s="105"/>
     </row>
@@ -4527,10 +4610,10 @@
       <c r="B91" s="106"/>
       <c r="D91" s="107"/>
       <c r="E91" s="59" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F91" s="64" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G91" s="139"/>
     </row>
@@ -4539,7 +4622,7 @@
       <c r="B92" s="106"/>
       <c r="E92" s="59"/>
       <c r="F92" s="64" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G92" s="140"/>
     </row>
@@ -4548,7 +4631,7 @@
       <c r="B93" s="106"/>
       <c r="E93" s="59"/>
       <c r="F93" s="64" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G93" s="141"/>
     </row>
@@ -4557,7 +4640,7 @@
       <c r="B94" s="106"/>
       <c r="E94" s="59"/>
       <c r="F94" s="64" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G94" s="142"/>
     </row>
@@ -4566,7 +4649,7 @@
       <c r="B95" s="106"/>
       <c r="E95" s="59"/>
       <c r="F95" s="64" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G95" s="107"/>
     </row>
@@ -4587,14 +4670,14 @@
     <row r="99" ht="15" customHeight="1" spans="1:7">
       <c r="A99" s="108"/>
       <c r="B99" s="109" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D99" s="110"/>
       <c r="E99" s="59" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F99" s="144" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G99" s="145"/>
     </row>
@@ -4603,7 +4686,7 @@
       <c r="B100" s="109"/>
       <c r="E100" s="59"/>
       <c r="F100" s="144" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G100" s="146"/>
     </row>
@@ -4612,10 +4695,10 @@
       <c r="B101" s="109"/>
       <c r="D101" s="66"/>
       <c r="E101" s="59" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F101" s="144" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G101" s="66"/>
     </row>
@@ -4624,7 +4707,7 @@
       <c r="B102" s="109"/>
       <c r="E102" s="59"/>
       <c r="F102" s="144" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G102" s="147"/>
     </row>
@@ -4633,10 +4716,10 @@
       <c r="B103" s="109"/>
       <c r="D103" s="111"/>
       <c r="E103" s="83" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F103" s="144" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G103" s="111"/>
     </row>
@@ -4645,10 +4728,10 @@
       <c r="B104" s="109"/>
       <c r="D104" s="26"/>
       <c r="E104" s="83" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F104" s="144" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G104" s="26"/>
     </row>
@@ -4657,10 +4740,10 @@
       <c r="B105" s="109"/>
       <c r="D105" s="112"/>
       <c r="E105" s="83" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F105" s="144" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G105" s="112"/>
     </row>
@@ -4681,14 +4764,14 @@
     <row r="109" ht="15" customHeight="1" spans="1:7">
       <c r="A109" s="113"/>
       <c r="B109" s="114" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D109" s="115"/>
       <c r="E109" s="59" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F109" s="144" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G109" s="149"/>
     </row>
@@ -4697,7 +4780,7 @@
       <c r="B110" s="114"/>
       <c r="E110" s="59"/>
       <c r="F110" s="144" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G110" s="115"/>
     </row>
@@ -4706,7 +4789,7 @@
       <c r="B111" s="114"/>
       <c r="E111" s="59"/>
       <c r="F111" s="144" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G111" s="150"/>
     </row>
@@ -4715,10 +4798,10 @@
       <c r="B112" s="114"/>
       <c r="D112" s="116"/>
       <c r="E112" s="59" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F112" s="144" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G112" s="116"/>
     </row>
@@ -4727,7 +4810,7 @@
       <c r="B113" s="114"/>
       <c r="E113" s="59"/>
       <c r="F113" s="144" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G113" s="61"/>
     </row>
@@ -4736,7 +4819,7 @@
       <c r="B114" s="114"/>
       <c r="E114" s="59"/>
       <c r="F114" s="144" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G114" s="151"/>
     </row>
@@ -4745,10 +4828,10 @@
       <c r="B115" s="114"/>
       <c r="D115" s="117"/>
       <c r="E115" s="59" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F115" s="144" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G115" s="117"/>
     </row>
@@ -4757,7 +4840,7 @@
       <c r="B116" s="114"/>
       <c r="E116" s="59"/>
       <c r="F116" s="144" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G116" s="152"/>
     </row>
@@ -4766,10 +4849,10 @@
       <c r="B117" s="114"/>
       <c r="D117" s="118"/>
       <c r="E117" s="83" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F117" s="144" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G117" s="118"/>
     </row>
@@ -4778,14 +4861,14 @@
     <row r="120" ht="3.75" customHeight="1"/>
     <row r="121" ht="15" customHeight="1" spans="2:7">
       <c r="B121" s="119" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D121" s="120"/>
       <c r="E121" s="59" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F121" s="144" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G121" s="120"/>
     </row>
@@ -4793,7 +4876,7 @@
       <c r="B122" s="119"/>
       <c r="E122" s="59"/>
       <c r="F122" s="144" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G122" s="153"/>
     </row>
@@ -4801,10 +4884,10 @@
       <c r="B123" s="119"/>
       <c r="D123" s="121"/>
       <c r="E123" s="59" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F123" s="144" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G123" s="154"/>
     </row>
@@ -4812,7 +4895,7 @@
       <c r="B124" s="119"/>
       <c r="E124" s="59"/>
       <c r="F124" s="144" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G124" s="155"/>
     </row>
@@ -4820,7 +4903,7 @@
       <c r="B125" s="119"/>
       <c r="E125" s="59"/>
       <c r="F125" s="144" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G125" s="156"/>
     </row>
@@ -4829,14 +4912,14 @@
     <row r="128" ht="3.75" customHeight="1"/>
     <row r="129" ht="15" customHeight="1" spans="2:7">
       <c r="B129" s="157" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D129" s="158"/>
       <c r="E129" s="59" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F129" s="159" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G129" s="158"/>
     </row>
@@ -4909,7 +4992,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00833333333333" defaultRowHeight="14.25" outlineLevelCol="5"/>
@@ -4924,22 +5007,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -4948,20 +5031,20 @@
         <v>CS1</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C34" si="1">LEFT(E2,5)</f>
         <v>CS1.1</v>
       </c>
       <c r="D2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -4970,20 +5053,20 @@
         <v>CS1</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="1"/>
         <v>CS1.1</v>
       </c>
       <c r="D3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -4992,20 +5075,20 @@
         <v>CS1</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="1"/>
         <v>CS1.2</v>
       </c>
       <c r="D4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -5014,20 +5097,20 @@
         <v>CS1</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="1"/>
         <v>CS1.2</v>
       </c>
       <c r="D5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -5036,20 +5119,20 @@
         <v>CS2</v>
       </c>
       <c r="B6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="1"/>
         <v>CS2.1</v>
       </c>
       <c r="D6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -5058,20 +5141,20 @@
         <v>CS2</v>
       </c>
       <c r="B7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="1"/>
         <v>CS2.1</v>
       </c>
       <c r="D7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -5080,20 +5163,20 @@
         <v>CS2</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="1"/>
         <v>CS2.1</v>
       </c>
       <c r="D8" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -5102,20 +5185,20 @@
         <v>CS2</v>
       </c>
       <c r="B9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="1"/>
         <v>CS2.2</v>
       </c>
       <c r="D9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -5124,20 +5207,20 @@
         <v>CS2</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="1"/>
         <v>CS2.2</v>
       </c>
       <c r="D10" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F10" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -5146,20 +5229,20 @@
         <v>CS3</v>
       </c>
       <c r="B11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="1"/>
         <v>CS3.1</v>
       </c>
       <c r="D11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -5168,20 +5251,20 @@
         <v>CS3</v>
       </c>
       <c r="B12" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="1"/>
         <v>CS3.1</v>
       </c>
       <c r="D12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -5190,20 +5273,20 @@
         <v>CS3</v>
       </c>
       <c r="B13" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="1"/>
         <v>CS3.2</v>
       </c>
       <c r="D13" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F13" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -5212,20 +5295,20 @@
         <v>CS3</v>
       </c>
       <c r="B14" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="1"/>
         <v>CS3.2</v>
       </c>
       <c r="D14" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F14" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -5234,20 +5317,20 @@
         <v>CS4</v>
       </c>
       <c r="B15" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="1"/>
         <v>CS4.1</v>
       </c>
       <c r="D15" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F15" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -5256,20 +5339,20 @@
         <v>CS4</v>
       </c>
       <c r="B16" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="1"/>
         <v>CS4.1</v>
       </c>
       <c r="D16" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F16" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -5278,20 +5361,20 @@
         <v>CS4</v>
       </c>
       <c r="B17" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="1"/>
         <v>CS4.1</v>
       </c>
       <c r="D17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F17" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -5300,20 +5383,20 @@
         <v>CS4</v>
       </c>
       <c r="B18" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="1"/>
         <v>CS4.2</v>
       </c>
       <c r="D18" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F18" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -5322,20 +5405,20 @@
         <v>CS4</v>
       </c>
       <c r="B19" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="1"/>
         <v>CS4.2</v>
       </c>
       <c r="D19" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F19" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -5344,20 +5427,20 @@
         <v>CS4</v>
       </c>
       <c r="B20" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="1"/>
         <v>CS4.3</v>
       </c>
       <c r="D20" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F20" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -5366,20 +5449,20 @@
         <v>CS4</v>
       </c>
       <c r="B21" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="1"/>
         <v>CS4.3</v>
       </c>
       <c r="D21" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F21" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -5388,20 +5471,20 @@
         <v>CS4</v>
       </c>
       <c r="B22" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="1"/>
         <v>CS4.4</v>
       </c>
       <c r="D22" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F22" t="s">
         <v>200</v>
-      </c>
-      <c r="F22" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -5410,20 +5493,20 @@
         <v>CS5</v>
       </c>
       <c r="B23" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="1"/>
         <v>CS5.1</v>
       </c>
       <c r="D23" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F23" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -5432,20 +5515,20 @@
         <v>CS5</v>
       </c>
       <c r="B24" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="1"/>
         <v>CS5.1</v>
       </c>
       <c r="D24" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F24" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -5454,20 +5537,20 @@
         <v>CS5</v>
       </c>
       <c r="B25" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="1"/>
         <v>CS5.1</v>
       </c>
       <c r="D25" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F25" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -5476,20 +5559,20 @@
         <v>CS5</v>
       </c>
       <c r="B26" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="1"/>
         <v>CS5.2</v>
       </c>
       <c r="D26" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E26" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F26" t="s">
         <v>210</v>
-      </c>
-      <c r="F26" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -5498,20 +5581,20 @@
         <v>CS6</v>
       </c>
       <c r="B27" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="1"/>
         <v>CS6.1</v>
       </c>
       <c r="D27" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F27" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -5520,20 +5603,20 @@
         <v>CS6</v>
       </c>
       <c r="B28" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="1"/>
         <v>CS6.1</v>
       </c>
       <c r="D28" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F28" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -5542,20 +5625,20 @@
         <v>CS6</v>
       </c>
       <c r="B29" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="1"/>
         <v>CS6.2</v>
       </c>
       <c r="D29" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E29" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F29" t="s">
         <v>218</v>
-      </c>
-      <c r="F29" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -5564,20 +5647,20 @@
         <v>CS6</v>
       </c>
       <c r="B30" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="1"/>
         <v>CS6.3</v>
       </c>
       <c r="D30" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E30" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F30" t="s">
         <v>220</v>
-      </c>
-      <c r="F30" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -5586,20 +5669,20 @@
         <v>CS6</v>
       </c>
       <c r="B31" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="1"/>
         <v>CS6.4</v>
       </c>
       <c r="D31" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F31" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -5608,20 +5691,20 @@
         <v>CS6</v>
       </c>
       <c r="B32" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="1"/>
         <v>CS6.4</v>
       </c>
       <c r="D32" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F32" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -5630,20 +5713,20 @@
         <v>CS6</v>
       </c>
       <c r="B33" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="1"/>
         <v>CS6.5</v>
       </c>
       <c r="D33" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F33" t="s">
         <v>227</v>
-      </c>
-      <c r="F33" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -5652,20 +5735,20 @@
         <v>CS6</v>
       </c>
       <c r="B34" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="1"/>
         <v>CS6.6</v>
       </c>
       <c r="D34" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E34" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F34" t="s">
         <v>229</v>
-      </c>
-      <c r="F34" t="s">
-        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -5698,22 +5781,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -5722,20 +5805,20 @@
         <v>US1</v>
       </c>
       <c r="B2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C54" si="1">LEFT(E2,5)</f>
         <v>US1.1</v>
       </c>
       <c r="D2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -5744,20 +5827,20 @@
         <v>US1</v>
       </c>
       <c r="B3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="1"/>
         <v>US1.1</v>
       </c>
       <c r="D3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -5766,20 +5849,20 @@
         <v>US1</v>
       </c>
       <c r="B4" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="1"/>
         <v>US1.1</v>
       </c>
       <c r="D4" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E4" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F4" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -5788,20 +5871,20 @@
         <v>US1</v>
       </c>
       <c r="B5" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="1"/>
         <v>US1.1</v>
       </c>
       <c r="D5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E5" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -5810,20 +5893,20 @@
         <v>US1</v>
       </c>
       <c r="B6" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="1"/>
         <v>US1.1</v>
       </c>
       <c r="D6" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E6" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F6" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -5832,20 +5915,20 @@
         <v>US1</v>
       </c>
       <c r="B7" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="1"/>
         <v>US1.1</v>
       </c>
       <c r="D7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E7" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F7" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -5854,20 +5937,20 @@
         <v>US1</v>
       </c>
       <c r="B8" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="1"/>
         <v>US1.1</v>
       </c>
       <c r="D8" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E8" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F8" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -5876,20 +5959,20 @@
         <v>US1</v>
       </c>
       <c r="B9" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="1"/>
         <v>US1.2</v>
       </c>
       <c r="D9" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E9" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F9" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -5898,20 +5981,20 @@
         <v>US1</v>
       </c>
       <c r="B10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="1"/>
         <v>US1.2</v>
       </c>
       <c r="D10" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E10" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="F10" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -5920,20 +6003,20 @@
         <v>US1</v>
       </c>
       <c r="B11" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="1"/>
         <v>US1.2</v>
       </c>
       <c r="D11" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E11" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F11" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -5942,20 +6025,20 @@
         <v>US1</v>
       </c>
       <c r="B12" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="1"/>
         <v>US1.2</v>
       </c>
       <c r="D12" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E12" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F12" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -5964,20 +6047,20 @@
         <v>US1</v>
       </c>
       <c r="B13" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="1"/>
         <v>US1.3</v>
       </c>
       <c r="D13" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E13" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F13" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -5986,20 +6069,20 @@
         <v>US1</v>
       </c>
       <c r="B14" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="1"/>
         <v>US1.3</v>
       </c>
       <c r="D14" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E14" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F14" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -6008,20 +6091,20 @@
         <v>US1</v>
       </c>
       <c r="B15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="1"/>
         <v>US1.4</v>
       </c>
       <c r="D15" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E15" t="s">
+        <v>267</v>
+      </c>
+      <c r="F15" t="s">
         <v>266</v>
-      </c>
-      <c r="F15" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -6030,20 +6113,20 @@
         <v>US2</v>
       </c>
       <c r="B16" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="1"/>
         <v>US2.1</v>
       </c>
       <c r="D16" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E16" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F16" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -6052,20 +6135,20 @@
         <v>US2</v>
       </c>
       <c r="B17" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="1"/>
         <v>US2.1</v>
       </c>
       <c r="D17" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E17" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F17" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -6074,20 +6157,20 @@
         <v>US2</v>
       </c>
       <c r="B18" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="1"/>
         <v>US2.1</v>
       </c>
       <c r="D18" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E18" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F18" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -6096,20 +6179,20 @@
         <v>US2</v>
       </c>
       <c r="B19" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="1"/>
         <v>US2.1</v>
       </c>
       <c r="D19" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E19" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F19" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -6118,20 +6201,20 @@
         <v>US2</v>
       </c>
       <c r="B20" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="1"/>
         <v>US2.1</v>
       </c>
       <c r="D20" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E20" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F20" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -6140,20 +6223,20 @@
         <v>US2</v>
       </c>
       <c r="B21" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="1"/>
         <v>US2.2</v>
       </c>
       <c r="D21" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E21" t="s">
+        <v>281</v>
+      </c>
+      <c r="F21" t="s">
         <v>280</v>
-      </c>
-      <c r="F21" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -6162,20 +6245,20 @@
         <v>US3</v>
       </c>
       <c r="B22" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="1"/>
         <v>US3.1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E22" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F22" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -6184,20 +6267,20 @@
         <v>US3</v>
       </c>
       <c r="B23" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="1"/>
         <v>US3.1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E23" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F23" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -6206,20 +6289,20 @@
         <v>US3</v>
       </c>
       <c r="B24" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="1"/>
         <v>US3.1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E24" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F24" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -6228,20 +6311,20 @@
         <v>US3</v>
       </c>
       <c r="B25" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="1"/>
         <v>US3.1</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E25" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F25" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -6250,20 +6333,20 @@
         <v>US3</v>
       </c>
       <c r="B26" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="1"/>
         <v>US3.1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E26" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F26" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -6272,20 +6355,20 @@
         <v>US3</v>
       </c>
       <c r="B27" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="1"/>
         <v>US3.1</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E27" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F27" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -6294,20 +6377,20 @@
         <v>US3</v>
       </c>
       <c r="B28" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="1"/>
         <v>US3.2</v>
       </c>
       <c r="D28" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E28" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F28" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -6316,20 +6399,20 @@
         <v>US3</v>
       </c>
       <c r="B29" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="1"/>
         <v>US3.2</v>
       </c>
       <c r="D29" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E29" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F29" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -6338,20 +6421,20 @@
         <v>US3</v>
       </c>
       <c r="B30" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="1"/>
         <v>US3.2</v>
       </c>
       <c r="D30" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E30" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F30" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -6360,20 +6443,20 @@
         <v>US3</v>
       </c>
       <c r="B31" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="1"/>
         <v>US3.2</v>
       </c>
       <c r="D31" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E31" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="F31" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -6382,20 +6465,20 @@
         <v>US3</v>
       </c>
       <c r="B32" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="1"/>
         <v>US3.2</v>
       </c>
       <c r="D32" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E32" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F32" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -6404,20 +6487,20 @@
         <v>US4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="1"/>
         <v>US4.1</v>
       </c>
       <c r="D33" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E33" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="F33" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -6426,20 +6509,20 @@
         <v>US4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="1"/>
         <v>US4.1</v>
       </c>
       <c r="D34" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E34" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F34" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -6448,20 +6531,20 @@
         <v>US4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="1"/>
         <v>US4.2</v>
       </c>
       <c r="D35" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E35" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F35" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -6470,20 +6553,20 @@
         <v>US4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="1"/>
         <v>US4.2</v>
       </c>
       <c r="D36" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E36" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="F36" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -6492,20 +6575,20 @@
         <v>US4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="1"/>
         <v>US4.3</v>
       </c>
       <c r="D37" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E37" t="s">
+        <v>319</v>
+      </c>
+      <c r="F37" t="s">
         <v>318</v>
-      </c>
-      <c r="F37" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -6514,20 +6597,20 @@
         <v>US4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="1"/>
         <v>US4.4</v>
       </c>
       <c r="D38" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E38" t="s">
+        <v>321</v>
+      </c>
+      <c r="F38" t="s">
         <v>320</v>
-      </c>
-      <c r="F38" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -6536,20 +6619,20 @@
         <v>US4</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="1"/>
         <v>US4.5</v>
       </c>
       <c r="D39" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E39" t="s">
+        <v>323</v>
+      </c>
+      <c r="F39" t="s">
         <v>322</v>
-      </c>
-      <c r="F39" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -6558,20 +6641,20 @@
         <v>US5</v>
       </c>
       <c r="B40" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="1"/>
         <v>US5.1</v>
       </c>
       <c r="D40" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E40" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F40" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -6580,20 +6663,20 @@
         <v>US5</v>
       </c>
       <c r="B41" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="1"/>
         <v>US5.1</v>
       </c>
       <c r="D41" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E41" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F41" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -6602,20 +6685,20 @@
         <v>US5</v>
       </c>
       <c r="B42" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="1"/>
         <v>US5.1</v>
       </c>
       <c r="D42" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E42" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F42" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -6624,20 +6707,20 @@
         <v>US5</v>
       </c>
       <c r="B43" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="1"/>
         <v>US5.2</v>
       </c>
       <c r="D43" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E43" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F43" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -6646,20 +6729,20 @@
         <v>US5</v>
       </c>
       <c r="B44" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="1"/>
         <v>US5.2</v>
       </c>
       <c r="D44" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E44" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F44" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -6668,20 +6751,20 @@
         <v>US5</v>
       </c>
       <c r="B45" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="1"/>
         <v>US5.2</v>
       </c>
       <c r="D45" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E45" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="F45" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -6690,20 +6773,20 @@
         <v>US5</v>
       </c>
       <c r="B46" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="1"/>
         <v>US5.3</v>
       </c>
       <c r="D46" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E46" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F46" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -6712,20 +6795,20 @@
         <v>US5</v>
       </c>
       <c r="B47" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="1"/>
         <v>US5.3</v>
       </c>
       <c r="D47" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E47" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="F47" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -6734,20 +6817,20 @@
         <v>US5</v>
       </c>
       <c r="B48" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="1"/>
         <v>US5.4</v>
       </c>
       <c r="D48" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E48" t="s">
+        <v>345</v>
+      </c>
+      <c r="F48" t="s">
         <v>344</v>
-      </c>
-      <c r="F48" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -6756,20 +6839,20 @@
         <v>US6</v>
       </c>
       <c r="B49" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="1"/>
         <v>US6.1</v>
       </c>
       <c r="D49" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E49" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F49" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -6778,20 +6861,20 @@
         <v>US6</v>
       </c>
       <c r="B50" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="1"/>
         <v>US6.1</v>
       </c>
       <c r="D50" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E50" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F50" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -6800,20 +6883,20 @@
         <v>US6</v>
       </c>
       <c r="B51" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="1"/>
         <v>US6.2</v>
       </c>
       <c r="D51" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E51" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F51" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -6822,20 +6905,20 @@
         <v>US6</v>
       </c>
       <c r="B52" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="1"/>
         <v>US6.2</v>
       </c>
       <c r="D52" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E52" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="F52" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -6844,20 +6927,20 @@
         <v>US6</v>
       </c>
       <c r="B53" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="1"/>
         <v>US6.2</v>
       </c>
       <c r="D53" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E53" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="F53" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -6866,20 +6949,20 @@
         <v>US7</v>
       </c>
       <c r="B54" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="1"/>
         <v>US7.0</v>
       </c>
       <c r="D54" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E54" t="s">
+        <v>360</v>
+      </c>
+      <c r="F54" t="s">
         <v>359</v>
-      </c>
-      <c r="F54" t="s">
-        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -6887,4 +6970,266 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr>
+    <tabColor theme="2"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="4" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="30.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>366</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr>
+    <tabColor theme="2"/>
+  </sheetPr>
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="11.25" customWidth="1"/>
+    <col min="2" max="2" width="41.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>386</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mise à jour du fichier nomenclature_OCS2d_2021_final.xlsx
</commit_message>
<xml_diff>
--- a/nomenclature/nomenclature_OCS2d_2021_final.xlsx
+++ b/nomenclature/nomenclature_OCS2d_2021_final.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowHeight="18435" tabRatio="574"/>
+    <workbookView windowHeight="17955" tabRatio="574"/>
   </bookViews>
   <sheets>
     <sheet name="Marque-Page-A5" sheetId="8" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="21P_HdF" sheetId="10" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Marque-Page-A5'!$A$55:$G$131</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Marque-Page-A5'!$A$1:$G$131</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -1634,9 +1634,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="35">
     <font>
@@ -1708,6 +1708,29 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -1715,16 +1738,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1738,6 +1753,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -1746,40 +1769,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1793,7 +1787,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1813,16 +1830,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1836,17 +1845,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2440,7 +2440,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2452,13 +2494,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2470,25 +2536,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2500,127 +2614,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2680,6 +2680,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -2709,26 +2724,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2748,17 +2754,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2780,138 +2780,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="104" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="111" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="102" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="92" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="120" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="93" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="110" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="121" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="119" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="115" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="118" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="117" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="117" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="110" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="115" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="116" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="112" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="112" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="109" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="107" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="108" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="108" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="91" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="114" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="106" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="104" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="105" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="94" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="95" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="106" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="100" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="119" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="111" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="113" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="98" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="101" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="121" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="102" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="101" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="105" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="114" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="103" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="96" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="120" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="113" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="109" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="103" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="97" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="97" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="100" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="116" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="118" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="107" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="103" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="94" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="98" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="97" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="93" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="95" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="96" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="99" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="91" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="92" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="99" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3666,12 +3666,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <tabColor theme="9" tint="-0.25"/>
-    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -4979,8 +4978,11 @@
     <mergeCell ref="F129:F131"/>
   </mergeCells>
   <pageMargins left="0.196850393700787" right="0.196850393700787" top="0.196850393700787" bottom="0.196850393700787" header="0.31496062992126" footer="0.31496062992126"/>
-  <pageSetup paperSize="11" scale="52" orientation="portrait"/>
+  <pageSetup paperSize="9" scale="75" orientation="portrait"/>
   <headerFooter/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="54" max="6" man="1"/>
+  </rowBreaks>
 </worksheet>
 </file>
 
@@ -5766,7 +5768,7 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00833333333333" defaultRowHeight="14.25" outlineLevelCol="5"/>
@@ -7043,7 +7045,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="1"/>

</xml_diff>